<commit_message>
improve search test case - better scenario
</commit_message>
<xml_diff>
--- a/docs/Test cases.xlsx
+++ b/docs/Test cases.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\valentina.morozova\PycharmProjects\DPG - PO pattern\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\valentina.morozova\PycharmProjects\Python-TA-Demonstration\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{916BFB7F-0923-4FB1-A864-4E9BA8E349CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA8F3C5B-8119-4FB2-80BA-46AEFC85D9E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{3B0F51DC-6901-4D6E-AC96-BA7EB52DA476}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{3B0F51DC-6901-4D6E-AC96-BA7EB52DA476}"/>
   </bookViews>
   <sheets>
     <sheet name="UI tests" sheetId="2" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="57">
   <si>
     <t>Test Case Name</t>
   </si>
@@ -115,24 +115,6 @@
   </si>
   <si>
     <t>The user with an existing address should be able to complete the order with all default options in the checkout process</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1. Open the main page. 
-2. Enter "computer" in the search panel.
-3. Click "Search" on the main page.
-4. Open "Advanced Search".
-5. Select "Computers &gt;&gt; Desktops" from the "Category" dropdown.
-6. Set the "Price range" to "From 800 to 1500".
-7. Click "Search" on the search page. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">1. Open the main page. 
-2. Enter "computer" in the search panel.
-3. Click "Search" on the main page.
-4. Open "Advanced Search".
-5. Select "Computers &gt;&gt; Desktops" from the "Category" dropdown.
-6. Set the "Price range" to "From 1000 to 1500".
-7. Click "Search" on the search page. </t>
   </si>
   <si>
     <t>Validate number of results for authors search</t>
@@ -235,16 +217,6 @@
 3)specified price ranges</t>
   </si>
   <si>
-    <t>1. There should be 4 products displayed for the initial search after step 3.
-2. There should be 3 products displayed for the advanced search after step 7.
-3. The first product in the advanced search should have the title "Build your own cheap computer".</t>
-  </si>
-  <si>
-    <t>1. There should be 4 products displayed for the initial search after step 3.
-2. There should be 1 product displayed for the advanced search after step 7.
-3. The product in the advanced search should have the title "Build your own computer".</t>
-  </si>
-  <si>
     <t>TC-UI-003.1</t>
   </si>
   <si>
@@ -284,6 +256,41 @@
       </rPr>
       <t>: B-UI-001</t>
     </r>
+  </si>
+  <si>
+    <t>1. Open the main page. 
+2. Enter "comput" in the search panel.
+3. Click "Search" on the main page.
+4. Open "Advanced Search".
+5. Select "Computers &gt;&gt; Desktops" from the "Category" dropdown.
+6. Click "Search" on the search page. 
+7. Set the "Price range" to "From 800 to 1500".
+8. Click "Search" on the search page.</t>
+  </si>
+  <si>
+    <t>1. Open the main page. 
+2. Enter "comput" in the search panel.
+3. Click "Search" on the main page.
+4. Open "Advanced Search".
+5. Select "Computers &gt;&gt; Desktops" from the "Category" dropdown.
+6. Click "Search" on the search page. 
+7. Set the "Price range" to "From 1000 to 1500".
+8. Click "Search" on the search page.</t>
+  </si>
+  <si>
+    <t>Test Case ID</t>
+  </si>
+  <si>
+    <t>1. There should be 6 products displayed for the initial search after step 3.
+2. There should be 4 products displayed for the search after step 6.
+3. There should be 3 products displayed for the search after step 8.
+4. The first product in the last search should have the title "Build your own cheap computer".</t>
+  </si>
+  <si>
+    <t>1. There should be 6 products displayed for the initial search after step 3.
+2. There should be 4 products displayed for the search after step 6.
+3. There should be 1 products displayed for the search after step 8.
+4. The first product in the last search should have the title "Build your own computer".</t>
   </si>
 </sst>
 </file>
@@ -707,6 +714,20 @@
         <scheme val="minor"/>
       </font>
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="1"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
     </dxf>
     <dxf>
       <font>
@@ -779,7 +800,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="1"/>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
           <color indexed="64"/>
@@ -808,7 +829,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="1"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
           <color indexed="64"/>
@@ -896,20 +917,6 @@
         <scheme val="minor"/>
       </font>
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="1"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
     </dxf>
     <dxf>
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="1"/>
@@ -928,19 +935,19 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{AE441058-1B94-4781-A832-DC73C74DAC96}" name="Table22" displayName="Table22" ref="A1:G7" totalsRowShown="0" headerRowDxfId="17" dataDxfId="9">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{AE441058-1B94-4781-A832-DC73C74DAC96}" name="Table22" displayName="Table22" ref="A1:G7" totalsRowShown="0" headerRowDxfId="17" dataDxfId="16">
   <autoFilter ref="A1:G7" xr:uid="{FF29ADA6-4548-4A7D-B14B-3A851166B6D3}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G3">
     <sortCondition ref="A1:A3"/>
   </sortState>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{B48E7F55-E36F-412D-B35D-283E13C2BEE5}" name="ID" dataDxfId="16"/>
-    <tableColumn id="2" xr3:uid="{6EF2DF52-A9CE-457F-BB49-C9E3B4E4E525}" name="Test Case Name" dataDxfId="15"/>
-    <tableColumn id="3" xr3:uid="{538235A3-491A-412F-AB0F-43703D79DA9A}" name="Feature" dataDxfId="14"/>
-    <tableColumn id="4" xr3:uid="{A5459528-547B-4EDA-BC4E-257870C08DDA}" name="Requirement" dataDxfId="13"/>
-    <tableColumn id="5" xr3:uid="{923475AA-662D-453B-9525-8083BAACE429}" name="Test Flow" dataDxfId="12"/>
-    <tableColumn id="6" xr3:uid="{80485CF0-0299-4D19-A9F7-0976B4B2762E}" name="Expected Result" dataDxfId="11"/>
-    <tableColumn id="7" xr3:uid="{8FAE8B35-46E8-41BB-A0CF-F01FC7822EFC}" name="Status" dataDxfId="10"/>
+    <tableColumn id="1" xr3:uid="{B48E7F55-E36F-412D-B35D-283E13C2BEE5}" name="Test Case ID" dataDxfId="15"/>
+    <tableColumn id="2" xr3:uid="{6EF2DF52-A9CE-457F-BB49-C9E3B4E4E525}" name="Test Case Name" dataDxfId="14"/>
+    <tableColumn id="3" xr3:uid="{538235A3-491A-412F-AB0F-43703D79DA9A}" name="Feature" dataDxfId="13"/>
+    <tableColumn id="4" xr3:uid="{A5459528-547B-4EDA-BC4E-257870C08DDA}" name="Requirement" dataDxfId="12"/>
+    <tableColumn id="5" xr3:uid="{923475AA-662D-453B-9525-8083BAACE429}" name="Test Flow" dataDxfId="11"/>
+    <tableColumn id="6" xr3:uid="{80485CF0-0299-4D19-A9F7-0976B4B2762E}" name="Expected Result" dataDxfId="10"/>
+    <tableColumn id="7" xr3:uid="{8FAE8B35-46E8-41BB-A0CF-F01FC7822EFC}" name="Status" dataDxfId="9"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1290,7 +1297,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.6640625" style="3" customWidth="1"/>
+    <col min="1" max="1" width="17.33203125" style="3" customWidth="1"/>
     <col min="2" max="3" width="18.77734375" style="3" customWidth="1"/>
     <col min="4" max="4" width="32.77734375" style="5" customWidth="1"/>
     <col min="5" max="6" width="42.77734375" style="3" customWidth="1"/>
@@ -1298,9 +1305,9 @@
     <col min="8" max="16384" width="8.88671875" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
-        <v>7</v>
+        <v>54</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>0</v>
@@ -1326,7 +1333,7 @@
         <v>12</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C2" s="7" t="s">
         <v>18</v>
@@ -1335,16 +1342,16 @@
         <v>22</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="G2" s="6" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A3" s="9" t="s">
         <v>15</v>
       </c>
@@ -1352,22 +1359,22 @@
         <v>13</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D3" s="10" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="E3" s="9" t="s">
-        <v>25</v>
+        <v>52</v>
       </c>
       <c r="F3" s="9" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="G3" s="9" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A4" s="6" t="s">
         <v>14</v>
       </c>
@@ -1375,16 +1382,16 @@
         <v>13</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>26</v>
+        <v>53</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
       <c r="G4" s="6" t="s">
         <v>6</v>
@@ -1392,7 +1399,7 @@
     </row>
     <row r="5" spans="1:7" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A5" s="9" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="B5" s="9" t="s">
         <v>16</v>
@@ -1404,10 +1411,10 @@
         <v>23</v>
       </c>
       <c r="E5" s="9" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="F5" s="9" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="G5" s="9" t="s">
         <v>6</v>
@@ -1415,7 +1422,7 @@
     </row>
     <row r="6" spans="1:7" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A6" s="11" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="B6" s="11" t="s">
         <v>16</v>
@@ -1427,16 +1434,16 @@
         <v>23</v>
       </c>
       <c r="E6" s="11" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="F6" s="11" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="G6" s="11" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="351.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" ht="343.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="13" t="s">
         <v>20</v>
       </c>
@@ -1444,16 +1451,16 @@
         <v>21</v>
       </c>
       <c r="C7" s="13" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D7" s="14" t="s">
         <v>24</v>
       </c>
       <c r="E7" s="13" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="F7" s="13" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="G7" s="13" t="s">
         <v>6</v>
@@ -1515,19 +1522,19 @@
         <v>8</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C2" s="7" t="s">
         <v>17</v>
       </c>
       <c r="D2" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="F2" s="6" t="s">
         <v>30</v>
-      </c>
-      <c r="E2" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="F2" s="6" t="s">
-        <v>32</v>
       </c>
       <c r="G2" s="6" t="s">
         <v>6</v>
@@ -1538,19 +1545,19 @@
         <v>9</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C3" s="10" t="s">
         <v>17</v>
       </c>
       <c r="D3" s="10" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="E3" s="9" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="F3" s="9" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="G3" s="9" t="s">
         <v>6</v>
@@ -1561,19 +1568,19 @@
         <v>10</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C4" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="D4" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="D4" s="7" t="s">
-        <v>31</v>
-      </c>
       <c r="E4" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="F4" s="6" t="s">
         <v>36</v>
-      </c>
-      <c r="F4" s="6" t="s">
-        <v>38</v>
       </c>
       <c r="G4" s="6" t="s">
         <v>6</v>
@@ -1584,19 +1591,19 @@
         <v>11</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C5" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="D5" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="D5" s="10" t="s">
-        <v>31</v>
-      </c>
       <c r="E5" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="F5" s="9" t="s">
         <v>37</v>
-      </c>
-      <c r="F5" s="9" t="s">
-        <v>39</v>
       </c>
       <c r="G5" s="9" t="s">
         <v>6</v>

</xml_diff>